<commit_message>
finished adding test plan
</commit_message>
<xml_diff>
--- a/test_plan.xlsx
+++ b/test_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dacot\WebstormProjects\P5-Web-Dev-Kanap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6060CB90-1A02-49C2-9895-6D759E40049A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6197F4-D541-4076-84ED-927AEA116724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54495" yWindow="-5385" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Feature</t>
   </si>
@@ -49,27 +49,18 @@
     <t>...</t>
   </si>
   <si>
-    <t>a user clicks a product</t>
-  </si>
-  <si>
     <t>Opens a product page</t>
   </si>
   <si>
     <t>displays selected product details</t>
   </si>
   <si>
-    <t>a user selects color</t>
-  </si>
-  <si>
     <t>drop down displays with option to select color</t>
   </si>
   <si>
     <t>color is selected</t>
   </si>
   <si>
-    <t>a user adds/removes quantity</t>
-  </si>
-  <si>
     <t>user clicks arrows to add/decrease quantity</t>
   </si>
   <si>
@@ -77,6 +68,93 @@
   </si>
   <si>
     <t>a user adds their product to cart</t>
+  </si>
+  <si>
+    <t>user clicks 'add to cart' button</t>
+  </si>
+  <si>
+    <t>product gets added to cart and navigates to cart.html</t>
+  </si>
+  <si>
+    <t>cart.html shows products user selected</t>
+  </si>
+  <si>
+    <t>A user views a product</t>
+  </si>
+  <si>
+    <t>a user selects a color for product</t>
+  </si>
+  <si>
+    <t>a user adds/removes the number of quantity for there product</t>
+  </si>
+  <si>
+    <t>cart.html loads displaying all items user has added to cart</t>
+  </si>
+  <si>
+    <t>User clicks 'cart' button or 'add to cart' button and cart.html loads</t>
+  </si>
+  <si>
+    <t>in cart.html, user can change quantity</t>
+  </si>
+  <si>
+    <t>quantity for a product increases or decreases in cart.html</t>
+  </si>
+  <si>
+    <t>in cart.html, user can increase/decrease number of quantity per product</t>
+  </si>
+  <si>
+    <t>In cart.html, user can remove item from there cart</t>
+  </si>
+  <si>
+    <t>in cart.html, user clicks delete button</t>
+  </si>
+  <si>
+    <t>the product associated with the delete buttom removes it from the cart (cart.html)</t>
+  </si>
+  <si>
+    <t>a user leaves a field empty</t>
+  </si>
+  <si>
+    <t>red outline appears in respective input field</t>
+  </si>
+  <si>
+    <t>In cart.html, first name, last name &amp; city must contain letters only. Input field should outline red if this condition is not met</t>
+  </si>
+  <si>
+    <t>a user enteres characters other than alphabetical letters in the firstName, LastName &amp; city fields</t>
+  </si>
+  <si>
+    <t>in cart.html, any input field should outline red when empty</t>
+  </si>
+  <si>
+    <t>in cart.html, email input field should follow convention of email</t>
+  </si>
+  <si>
+    <t>a user doesn’t input a valid email address</t>
+  </si>
+  <si>
+    <t>in cart.html, order button should validate each input field and display outline red when all above conditions of the input fields are not met.</t>
+  </si>
+  <si>
+    <t>a user clicks the order button</t>
+  </si>
+  <si>
+    <t>red outline appears in each respective input field, if conditions described above are not met.</t>
+  </si>
+  <si>
+    <t>in cart.html, if input fields pass conditions above, then order is processed and confirmation.html loads</t>
+  </si>
+  <si>
+    <t>order is processed and confirmation.html loads</t>
+  </si>
+  <si>
+    <t>in confirmation.html page, order Id should display, confirming order</t>
+  </si>
+  <si>
+    <t>a user loads the confirmation.html page</t>
+  </si>
+  <si>
+    <t>should see confirmation.html page loaded displaying order id.</t>
   </si>
 </sst>
 </file>
@@ -355,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -372,15 +450,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -404,6 +473,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,17 +710,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="3" width="58.42578125" customWidth="1"/>
-    <col min="4" max="4" width="57.85546875" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" customWidth="1"/>
     <col min="5" max="5" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -656,190 +743,242 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="D4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
+      <c r="C7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" ht="54" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>